<commit_message>
Edits to return the humanSubjects and experimentFiles on a per experiment basis. Main bug fixes were bringing into alignment with existing metadata landing pages NotSpecified, as well as providing unstained reagent, and north american adult cohort arm
</commit_message>
<xml_diff>
--- a/ImmPort/CompletedTemplates/Reagent_Sets.xlsx
+++ b/ImmPort/CompletedTemplates/Reagent_Sets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drach\Documents\AlphaBeta\ImmPort\CompletedTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB89F56B-A010-412B-BC4F-4A0871CAE655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4297A5EA-160A-4945-A627-E5888D06BE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="195" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reagent_Sets.txt" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>reagent_sets</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>Full panel with unloaded/negative tetramer controls for the NKT and MAIT specific tetramers</t>
+  </si>
+  <si>
+    <t>Unstained</t>
+  </si>
+  <si>
+    <t>Unstained Cells</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -652,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,13 +759,23 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>

</xml_diff>